<commit_message>
Print stmts for visibility and control for blank (np.nan) values
</commit_message>
<xml_diff>
--- a/fileOutput.xlsx
+++ b/fileOutput.xlsx
@@ -46,49 +46,49 @@
     <t>Master Jiraya</t>
   </si>
   <si>
-    <t>hmzmaabgom@calaa.irB</t>
-  </si>
-  <si>
-    <t>laocmmmnie@gernd.las</t>
-  </si>
-  <si>
-    <t>oeimim@mcgla.gna</t>
-  </si>
-  <si>
-    <t>ociingm@dgaom.elw</t>
-  </si>
-  <si>
-    <t>lcasmiormgre@mitay.aaj</t>
-  </si>
-  <si>
-    <t>50-204-5000329</t>
-  </si>
-  <si>
-    <t>59-004-3000522</t>
-  </si>
-  <si>
-    <t>05-204-9030250</t>
-  </si>
-  <si>
-    <t>04-000-5532902</t>
-  </si>
-  <si>
-    <t>00-252-0350490</t>
-  </si>
-  <si>
-    <t>sset/anetdmp/edyrr</t>
-  </si>
-  <si>
-    <t>anse/mdeyspd/rertt</t>
-  </si>
-  <si>
-    <t>drne/rmpssyt/eaetd</t>
-  </si>
-  <si>
-    <t>atns/etrydms/deper</t>
-  </si>
-  <si>
-    <t>ernt/demryta/esspd</t>
+    <t>aaimzbrgoa@aclBa.mhm</t>
+  </si>
+  <si>
+    <t>agelnlcesn@dmmor.iam</t>
+  </si>
+  <si>
+    <t>glicom@mmane.agi</t>
+  </si>
+  <si>
+    <t>nmmeidw@aogig.lco</t>
+  </si>
+  <si>
+    <t>yremcomsaiam@gtrij.aal</t>
+  </si>
+  <si>
+    <t>04-203-5005902</t>
+  </si>
+  <si>
+    <t>90-005-3245020</t>
+  </si>
+  <si>
+    <t>40-900-2203550</t>
+  </si>
+  <si>
+    <t>40-020-5029350</t>
+  </si>
+  <si>
+    <t>20-050-2095304</t>
+  </si>
+  <si>
+    <t>yssa/rndmtdr/peeet</t>
+  </si>
+  <si>
+    <t>pyta/tmersdd/rnsee</t>
+  </si>
+  <si>
+    <t>smnp/ardettd/eresy</t>
+  </si>
+  <si>
+    <t>tedp/aystres/rdemn</t>
+  </si>
+  <si>
+    <t>yend/esedrsm/rtatp</t>
   </si>
   <si>
     <t>Active</t>

</xml_diff>

<commit_message>
Updated script to have dynamic input path
</commit_message>
<xml_diff>
--- a/fileOutput.xlsx
+++ b/fileOutput.xlsx
@@ -46,49 +46,49 @@
     <t>Master Jiraya</t>
   </si>
   <si>
-    <t>aaimzbrgoa@aclBa.mhm</t>
-  </si>
-  <si>
-    <t>agelnlcesn@dmmor.iam</t>
-  </si>
-  <si>
-    <t>glicom@mmane.agi</t>
-  </si>
-  <si>
-    <t>nmmeidw@aogig.lco</t>
-  </si>
-  <si>
-    <t>yremcomsaiam@gtrij.aal</t>
-  </si>
-  <si>
-    <t>04-203-5005902</t>
-  </si>
-  <si>
-    <t>90-005-3245020</t>
-  </si>
-  <si>
-    <t>40-900-2203550</t>
-  </si>
-  <si>
-    <t>40-020-5029350</t>
-  </si>
-  <si>
-    <t>20-050-2095304</t>
-  </si>
-  <si>
-    <t>yssa/rndmtdr/peeet</t>
-  </si>
-  <si>
-    <t>pyta/tmersdd/rnsee</t>
-  </si>
-  <si>
-    <t>smnp/ardettd/eresy</t>
-  </si>
-  <si>
-    <t>tedp/aystres/rdemn</t>
-  </si>
-  <si>
-    <t>yend/esedrsm/rtatp</t>
+    <t>groblaiaaa@czamm.hmB</t>
+  </si>
+  <si>
+    <t>legemnimma@crnao.sdl</t>
+  </si>
+  <si>
+    <t>lgmmma@oeiin.cag</t>
+  </si>
+  <si>
+    <t>oncgeig@dwlao.imm</t>
+  </si>
+  <si>
+    <t>trasylgmejai@cmaro.iam</t>
+  </si>
+  <si>
+    <t>34-092-5500200</t>
+  </si>
+  <si>
+    <t>20-029-0503504</t>
+  </si>
+  <si>
+    <t>55-003-9400022</t>
+  </si>
+  <si>
+    <t>50-050-4200923</t>
+  </si>
+  <si>
+    <t>92-040-5253000</t>
+  </si>
+  <si>
+    <t>srtd/ermtend/seyap</t>
+  </si>
+  <si>
+    <t>nsre/paedtte/sdyrm</t>
+  </si>
+  <si>
+    <t>setr/nemtrds/aypde</t>
+  </si>
+  <si>
+    <t>sade/rtmsyre/dpten</t>
+  </si>
+  <si>
+    <t>tsdt/yerrpae/dmnse</t>
   </si>
   <si>
     <t>Active</t>

</xml_diff>